<commit_message>
feat: add signing officer PKKN
</commit_message>
<xml_diff>
--- a/referensi/referensi_pic_kl.xlsx
+++ b/referensi/referensi_pic_kl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10201"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4915ba6f4734bb40/Pekerjaan BMN/05. 2025/07_pengembangan_aplikasi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yusufpradana/Documents/apps/bar/referensi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{75967BF2-9330-024F-9807-22EE856793FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E6BA7B9-2635-B94C-BDB9-E8ABA636B68C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A115B16-6772-6941-A549-1EAD91F82FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3080" yWindow="3760" windowWidth="25640" windowHeight="14240" xr2:uid="{BB7DD76F-B0A1-0446-A17A-8D427D58188D}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="132">
   <si>
-    <t>kd_kl</t>
-  </si>
-  <si>
     <t>III-C</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>direktorat</t>
+  </si>
+  <si>
+    <t>kode_ba</t>
   </si>
 </sst>
 </file>
@@ -813,40 +813,40 @@
   <dimension ref="A1:E111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
         <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" t="s">
-        <v>124</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -854,16 +854,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -871,16 +871,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -888,16 +888,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -905,16 +905,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" t="s">
         <v>123</v>
-      </c>
-      <c r="D6" t="s">
-        <v>124</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -922,16 +922,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" t="s">
         <v>123</v>
-      </c>
-      <c r="D7" t="s">
-        <v>124</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -939,16 +939,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -956,16 +956,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -973,16 +973,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -990,16 +990,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -1007,16 +1007,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -1024,16 +1024,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1041,16 +1041,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E14">
         <v>3</v>
@@ -1058,16 +1058,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1075,16 +1075,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1092,16 +1092,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D17" t="s">
         <v>123</v>
-      </c>
-      <c r="D17" t="s">
-        <v>124</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" t="s">
         <v>128</v>
-      </c>
-      <c r="D18" t="s">
-        <v>129</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1126,16 +1126,16 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1143,16 +1143,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -1160,16 +1160,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -1177,16 +1177,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E22">
         <v>2</v>
@@ -1194,16 +1194,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -1211,16 +1211,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1228,16 +1228,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -1245,16 +1245,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1262,16 +1262,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E27">
         <v>2</v>
@@ -1279,16 +1279,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" t="s">
         <v>128</v>
-      </c>
-      <c r="D28" t="s">
-        <v>129</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1296,16 +1296,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D29" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -1313,16 +1313,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1330,16 +1330,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1347,16 +1347,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1364,16 +1364,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1381,16 +1381,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1398,16 +1398,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E35">
         <v>2</v>
@@ -1415,16 +1415,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36">
         <v>2</v>
@@ -1432,16 +1432,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1449,16 +1449,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1466,16 +1466,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -1483,16 +1483,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C40" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1500,16 +1500,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1517,16 +1517,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E42">
         <v>3</v>
@@ -1534,16 +1534,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D43" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -1551,16 +1551,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -1568,16 +1568,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D45" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -1585,16 +1585,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -1602,16 +1602,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -1619,16 +1619,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1636,16 +1636,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E49">
         <v>1</v>
@@ -1653,16 +1653,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1670,16 +1670,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E51">
         <v>2</v>
@@ -1687,16 +1687,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -1704,16 +1704,16 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E53">
         <v>2</v>
@@ -1721,16 +1721,16 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D54" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -1738,16 +1738,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1755,16 +1755,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E56">
         <v>3</v>
@@ -1772,16 +1772,16 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" t="s">
         <v>128</v>
-      </c>
-      <c r="D57" t="s">
-        <v>129</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -1789,16 +1789,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E58">
         <v>2</v>
@@ -1806,16 +1806,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" t="s">
         <v>128</v>
-      </c>
-      <c r="D59" t="s">
-        <v>129</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -1823,16 +1823,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D60" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E60">
         <v>3</v>
@@ -1840,16 +1840,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1857,16 +1857,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D62" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -1874,16 +1874,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E63">
         <v>3</v>
@@ -1891,16 +1891,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -1908,16 +1908,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -1925,16 +1925,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E66">
         <v>2</v>
@@ -1942,16 +1942,16 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D67" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -1959,16 +1959,16 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E68">
         <v>2</v>
@@ -1976,16 +1976,16 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C69" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -1993,16 +1993,16 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D70" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2010,16 +2010,16 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D71" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2027,16 +2027,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C72" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" t="s">
         <v>128</v>
-      </c>
-      <c r="D72" t="s">
-        <v>129</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2044,16 +2044,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C73" t="s">
+        <v>122</v>
+      </c>
+      <c r="D73" t="s">
         <v>123</v>
-      </c>
-      <c r="D73" t="s">
-        <v>124</v>
       </c>
       <c r="E73">
         <v>3</v>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D74" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E74">
         <v>2</v>
@@ -2078,16 +2078,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D75" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E75">
         <v>3</v>
@@ -2095,16 +2095,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D76" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E76">
         <v>2</v>
@@ -2112,16 +2112,16 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D77" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E77">
         <v>3</v>
@@ -2129,16 +2129,16 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C78" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" t="s">
         <v>128</v>
-      </c>
-      <c r="D78" t="s">
-        <v>129</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -2146,16 +2146,16 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D79" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E79">
         <v>2</v>
@@ -2163,16 +2163,16 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D80" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E80">
         <v>2</v>
@@ -2180,16 +2180,16 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C81" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81" t="s">
         <v>123</v>
-      </c>
-      <c r="D81" t="s">
-        <v>124</v>
       </c>
       <c r="E81">
         <v>3</v>
@@ -2197,16 +2197,16 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D82" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -2214,16 +2214,16 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D83" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -2231,16 +2231,16 @@
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E84">
         <v>1</v>
@@ -2248,16 +2248,16 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D85" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E85">
         <v>3</v>
@@ -2265,16 +2265,16 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2282,16 +2282,16 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2299,16 +2299,16 @@
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D88" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2316,16 +2316,16 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C89" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D89" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E89">
         <v>2</v>
@@ -2333,16 +2333,16 @@
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C90" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -2350,16 +2350,16 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D91" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E91">
         <v>2</v>
@@ -2367,16 +2367,16 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C92" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D92" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E92">
         <v>3</v>
@@ -2384,16 +2384,16 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D93" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E93">
         <v>3</v>
@@ -2401,16 +2401,16 @@
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D94" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E94">
         <v>3</v>
@@ -2418,16 +2418,16 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -2435,16 +2435,16 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C96" t="s">
+        <v>122</v>
+      </c>
+      <c r="D96" t="s">
         <v>123</v>
-      </c>
-      <c r="D96" t="s">
-        <v>124</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -2452,16 +2452,16 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D97" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E97">
         <v>2</v>
@@ -2469,16 +2469,16 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D98" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E98">
         <v>1</v>
@@ -2486,16 +2486,16 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -2503,16 +2503,16 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D100" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E100">
         <v>2</v>
@@ -2520,16 +2520,16 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D101" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E101">
         <v>2</v>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C102" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D102" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E102">
         <v>3</v>
@@ -2554,16 +2554,16 @@
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D103" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E103">
         <v>3</v>
@@ -2571,16 +2571,16 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C104" t="s">
+        <v>122</v>
+      </c>
+      <c r="D104" t="s">
         <v>123</v>
-      </c>
-      <c r="D104" t="s">
-        <v>124</v>
       </c>
       <c r="E104">
         <v>3</v>
@@ -2588,16 +2588,16 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D105" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E105">
         <v>3</v>
@@ -2605,16 +2605,16 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C106" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D106" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E106">
         <v>1</v>
@@ -2622,16 +2622,16 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D107" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E107">
         <v>3</v>
@@ -2639,16 +2639,16 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C108" t="s">
+        <v>127</v>
+      </c>
+      <c r="D108" t="s">
         <v>128</v>
-      </c>
-      <c r="D108" t="s">
-        <v>129</v>
       </c>
       <c r="E108">
         <v>1</v>
@@ -2656,16 +2656,16 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C109" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D109" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E109">
         <v>3</v>
@@ -2673,16 +2673,16 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D110" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E110">
         <v>3</v>

</xml_diff>